<commit_message>
view table with duplicated mark
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
   <si>
     <t>#ref</t>
   </si>
@@ -62,101 +62,106 @@
     <t>Abstract</t>
   </si>
   <si>
-    <t>ACM DL</t>
-  </si>
-  <si>
-    <t>10.1145/2460999.2461025</t>
-  </si>
-  <si>
-    <t>Imtiaz, Salma , Bano, Muneera , Ikram, Naveed , Niazi, Mahmood</t>
-  </si>
-  <si>
-    <t>A Tertiary Study: Experiences of Conducting Systematic Literature Reviews in Software Engineering</t>
-  </si>
-  <si>
-    <t>Proceedings of the 17th International Conference on Evaluation and Assessment in Software Engineering</t>
-  </si>
-  <si>
-    <t>inproceedings</t>
+    <t>Web of Science</t>
+  </si>
+  <si>
+    <t>10.1109er/COMPSAC48688.2020.0-122</t>
+  </si>
+  <si>
+    <t>R. Fáçtima , A. Yasin , L. Liu , J. Wang</t>
+  </si>
+  <si>
+    <t>Google Scholar vs. Dblp vs. Microsoft Academic Search: An Indexing Comparison for Software Engineering Literature</t>
+  </si>
+  <si>
+    <t>2020 IEEE 44th Annuál Computers, Software, and Applications Conference (COMPSAC)</t>
+  </si>
+  <si>
+    <t>INPROCEEDINGS</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>177–182</t>
-  </si>
-  <si>
-    <t>empirical software engineering, experiences, tertiary study, lessons learnt, systematic literature reviews</t>
-  </si>
-  <si>
-    <t>Context: The use of Systematic Literature Review (SLR) requires expertise and poses many challenges for novice researchers. The experiences of those who have used this research methodology can benefit novice researchers in effectively dealing with these challenges. Objective: The aim of this study is to record the reported experiences of conducting Systematic Literature Reviews, for the benefit of new researchers. Such a 
-review will greatly benefit the researchers wanting to conduct SLR for the very first time. Method: We conducted a tertiary study to gather the experiences published by researchers. Studies that have used the SLR research methodology in software engineering and have implicitly or explicitly reported their experiences are included in this review. Results: Our research has revealed 116 studies relevant to the theme. The data has been extracted by two researchers working independently and conflicts resolved after discussion with third researcher. Findings from these studies highlight Search Strategy, Online Databases, Planning and Data Extraction as the most challenging phases of SLR. Lack of standard terminology in software engineering papers, poor quality of abstracts and problems with search engines are some of the most cited challenges. Conclusion: Further research and guidelines is required to facilitate novice researchers in conducting these phases properly.</t>
-  </si>
-  <si>
-    <t>10.1145/3425269.3425277</t>
-  </si>
-  <si>
-    <t>Costa, Diego Ivo Campos , Filho, Eduardo Pereira e Silva , Silva, Reginaldo Florencio da , de C. Quaresma Gama, Thiago Dias , Cort\'es, Mariela I.</t>
-  </si>
-  <si>
-    <t>Microservice Architecture: A Tertiary Study</t>
-  </si>
-  <si>
-    <t>Proceedings of the 14th Brazilian Symposium on Software Components, Architectures, and Reuse</t>
-  </si>
-  <si>
-    <t>61–70</t>
-  </si>
-  <si>
-    <t>Mapeamento sistem\'atico, Padr\~oes de arquitetura, Microsservi\ccos, Academia, Industria, Arquitetura de software</t>
-  </si>
-  <si>
-    <t>Context. The large-scale use of microservices and their increasing adoption in the industry in recent years has motivated researches 
-on the most diverse aspects related to microservice-based development. However, as it is a relatively new topic, there is still no consolidated body of knowledge in the area. Objective. The present work intends to investigate the current state of research on microservices based on the formulation of six research questions covering fundamental aspects, such as: main interest topics and adopted standards, techniques and tools have been used and application areas. Method. From four digital libraries, 22 secondary studies were selected as a data source, which were analyzed and synthesized in the present study following the proposed research protocol. Results. Among the main topics of interest addressed, we highlight researches related to the applicability of microservice architecture, both by industry and academia. Results indicated that standards focus on challenges related to communication have been the most commonly considered by researchers of the area. Finally, the predominance in the use of the Docker container and the presence of DevOps practices in the automation of operations are noteworthy. Conclusions. The present mapping study points to some directions of research based on the identified gaps, such as modeling and 
-testing of microservice applications, and addressing security aspects. Another promising point to be explored involves the combined use of microservice architecture with other related concepts such as IoT, smart cities, 
-FOG computing and reactive systems, in order to reinforce the use of microservices, as well as creating new solutions and challenges to be researched.</t>
-  </si>
-  <si>
-    <t>10.1145/3106195.3106212</t>
-  </si>
-  <si>
-    <t>Marimuthu, C. , Chandrasekaran, K.</t>
-  </si>
-  <si>
-    <t>Systematic Studies in Software Product Lines: A Tertiary Study</t>
-  </si>
-  <si>
-    <t>Proceedings of the 21st International Systems and Software 
-Product Line Conference - Volume A</t>
-  </si>
-  <si>
-    <t>143–152</t>
-  </si>
-  <si>
-    <t>systematic review, software product line, tertiary study</t>
-  </si>
-  <si>
-    <t>Software product lines are widely used in the software industries to increase the re-usability and to decrease maintenance cost. On the other hand, systematic reviews are widely used in the software engineering research community to provide the overview of the research field and practitioners guidelines. Researchers have conducted many systematic studies on the different aspects of SPLs. To the best of our knowledge, till now there is no tertiary study conducted on systematic studies of SPL related research topics. In this paper, we aim at conducting a systematic mapping study of existing systematic studies to report the overview of the findings for researchers and practitioners. We performed snowballing and automated search to find out the relevant systematic studies. As a result, we analyzed 60 relevant studies to answer 5 research questions. The main focus of this tertiary study is to highlight the research topics, type of published reviews, active researchers and publication forums. Additionally, we highlight some of the limitations of the systematic studies. The important finding of this study is that the research field is well matured as the systematic studies covered a wide range of research topics. Another important finding is that many studies provided information for practitioners as well as researchers which is a notable improvement in the systematic reviews. However, many studies failed to assess the quality of 
-the primary studies which is the major limitation of the existing systematic studies.</t>
-  </si>
-  <si>
-    <t>10.1145/2745802.2745815</t>
-  </si>
-  <si>
-    <t>Zhou, You , Zhang, He , Huang, Xin , Yang, Song , Babar, Muhammad Ali , Tang, Hao</t>
-  </si>
-  <si>
-    <t>Quality Assessment of Systematic Reviews in Software Engineering: A Tertiary Study</t>
-  </si>
-  <si>
-    <t>Proceedings of the 19th International Conference on Evaluation and Assessment in Software Engineering</t>
-  </si>
-  <si>
-    <t>software engineering, quality assessment, systematic (literature) review</t>
-  </si>
-  <si>
-    <t>Context: The quality of an Systematic Literature Review (SLR) is as good as the quality of the reviewed papers. Hence, it is vital to rigorously assess the papers included in an SLR. There has been no tertiary study aimed at reporting the state of the practice of quality assessment used in SLRs in Software Engineering (SE).Objective: We aimed to study the practices of quality assessment of the papers included in SLRs in SE.Method: We conducted a tertiary study of the SLRs that have performed quality assessment of the reviewed papers.Results: We identified and analyzed different aspects of the quality assessment of the papers included in 127 SLRs.Conclusion: Researchers use a variety of strategies for quality assessment of the papers reviewed, but report little about the justification for the used criteria. The focus is creditability but not relevance 
-aspect of the papers. Appropriate guidelines are required for devising quality assessment strategies.</t>
+    <t>1097-1098</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>ewrer</t>
+  </si>
+  <si>
+    <t>Gáogle;Systematics;Software engineering;Software;Bibliographies;Search engines;Indexing;Search Engines;Google Scholar;dblp;Microsoft Academic Search;Software Engineering;Indexing;Tertiary Study;Mapping Study</t>
+  </si>
+  <si>
+    <t>Bááckground: One of the necessary conditions for any substantial research work is to synthesis the depth and the breath of the existing published literature on that topic. It is, thus, of extreme importance for a researcher to understand and look for both credible and exhaustive information sources. This first (important) step can be made significantly easier if the researcher can employ a more systematic way to extract the maximum of the literature on the topic. Objective: Essentially, the objective of this preliminary study is to rank three freely available academic search engines (Google Scholar, DBLP, Microsoft Academic Search) on the basis of the indexed Software Engineering academic literature they contain. Method: We have used a systematic mapping to conduct the study. Results: After extracting and analyzing 1067 secondary studies (from 18 tertiary studies), we have concluded that Google Scholar has indexed 98.96%, DBLP has indexed 93.43%, and Microsoft Academic Search engine has indexed 97.46% of the secondary studies. Thus, this implies that Google Scholar and Microsoft Academic Search might be a better-suited option for searching for secondary studies.</t>
+  </si>
+  <si>
+    <t>IEEE Xplore</t>
+  </si>
+  <si>
+    <t>10.1109/ICGSE.2012.29</t>
+  </si>
+  <si>
+    <t>A. B. Marques , R. Rodrigues , T. Conte</t>
+  </si>
+  <si>
+    <t>Systematic Literature Reviews in Distributed Software Development: A Tertiary Study</t>
+  </si>
+  <si>
+    <t>2012 IEEE Seventh International Conference on Global Software Engineering</t>
+  </si>
+  <si>
+    <t>134-143</t>
+  </si>
+  <si>
+    <t>6337350</t>
+  </si>
+  <si>
+    <t>computer science education;formal specification;groupware;reviews;software engineering;distributed software development;DSD;geographically distant customers;global customers;systematic literature reviews;SLR;tertiary review;distributed development management;software requirements;software design;software engineering education;organizations;Systematics;Software;Software engineering;Collaboration;Research and development management;Organizations;Context;Distributed Software Development;Global Software Engineering;Empirical Evidence;Systematic Review;Tertiary Study</t>
+  </si>
+  <si>
+    <t>Distributed Software Development (DSD) emerged from the need to achieve geographically distant customers and currently, allows organizations have global customers and other benefits. This scenario has given rise to new Software Engineering challenges resulting from DSD particularities. Several Systematic Reviews were conducted to address these new challenges. The objective of this paper is to categorize systematic reviews conducted in DSD context. We used the systematic review method to identify SLRs (Systematic Literature Reviews) that address DSD aspects. This study is categorized as a tertiary review. Of fourteen SLRs, seven address aspects of managing distributed development. Four SLRs addressed topics of engineering process. The three remaining are related to Requirements, Design and Software Engineering Education in DSD. The topic areas covered by SLRs are limited, where the majority are focused on summarize the current knowledge concerning a research question. Despite the number of SLRs, the amount of empirical studies is relatively small.</t>
+  </si>
+  <si>
+    <t>10.1109/ACCESS.2020.2971712</t>
+  </si>
+  <si>
+    <t>A. Yasin , R. Fatima , L. Wen , W. Afzal , M. Azhar , R. Torkar</t>
+  </si>
+  <si>
+    <t>On Using Grey Literature and Google Scholar in Systematic Literature Reviews in Software Engineering</t>
+  </si>
+  <si>
+    <t>IEEE Access</t>
+  </si>
+  <si>
+    <t>ARTICLE</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>36226-36243</t>
+  </si>
+  <si>
+    <t>8984351</t>
+  </si>
+  <si>
+    <t>grey systems;Internet;search engines;software engineering;software reviews;Google Scholar;systematic mapping study;grey literature;systematic literature reviews;Software Engineering;quality checklist;tertiary study;search engine;Systematics;Google;Software engineering;Bibliographies;Internet;Databases;Guidelines;Grey literature;Google scholar;software engineering;empirical evaluation;systematic mapping;tertiary study;gray;quality checklist</t>
+  </si>
+  <si>
+    <t>Context: The inclusion of grey literature (GL) is important to remove publication bias while gathering available evidence regarding a certain topic. The number of systematic literature reviews (SLRs) in Software Engineering (SE) is increasing but we do not know about the extent of GL usage in these SLRs. Moreover, Google Scholar is rapidly becoming a search engine of choice for many researchers but the extent to which it can find the primary studies is not known. Objective: This tertiary study is an attempt to i) measure the usage of GL in SLRs in SE. Furthermore this study proposes strategies for categorizing GL and a quality checklist to use for GL in future SLRs; ii) explore if it is feasible to use only Google Scholar for finding scholarly articles for academic research. Method: We have conducted a systematic mapping study to measure the extent of GL usage in SE SLRs as well as to measure the feasibility of finding primary studies using Google Scholar. Results and conclusions: a) Grey Literature: 76.09% SLRs (105 out of 138) in SE have included one or more GL studies as primary studies. Among total primary studies across all SLRs (6307), 582 are classified as GL, making the frequency of GL citing as 9.23%. The intensity of GL use indicate that each SLR contains 5 primary studies on average (total intensity of GL use being 5.54). The ranking of GL tells us that conference papers are the most used form 43.3% followed by technical reports 28.52%. Universities, research institutes, labs and scientific societies together make up 67.7% of GL used, indicating that these are useful sources for searching GL. We additionally propose strategies for categorizing GL and criteria for evaluating GL quality, which can become a basis for more detailed guidelines for including GL in future SLRs. b) Google Scholar Results: The results show that Google Scholar was able to retrieve 96% of primary studies of these SLRs. Most of the primary studies that were not found using Google Scholar were from grey sources.</t>
+  </si>
+  <si>
+    <t>10.1109/ACCESS.2022.2971712</t>
+  </si>
+  <si>
+    <t>8984352</t>
+  </si>
+  <si>
+    <t>Scopus</t>
   </si>
 </sst>
 </file>
@@ -208,27 +213,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="6.02734375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.0625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="14.79296875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="6.5859375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="25.296875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="128.58984375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="89.23828125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="94.7109375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.61328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="36.37890625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="53.78125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="104.7578125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="78.296875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="15.84765625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="14.0390625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="10.3828125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="8.82421875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="12.86328125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="10.875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="13.70703125" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="25.296875" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="106.4375" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="10.60546875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="255.0" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="255.0" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -290,7 +295,7 @@
         <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>2013.0</v>
+        <v>2020.0</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -315,40 +320,40 @@
         <v>23</v>
       </c>
       <c r="L2"/>
-      <c r="M2" t="n">
-        <v>6.0</v>
+      <c r="M2" t="s">
+        <v>24</v>
       </c>
       <c r="N2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="O2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="P2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.0</v>
+        <v>101.0</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C3" t="n">
-        <v>2020.0</v>
+        <v>2012.0</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
@@ -358,110 +363,212 @@
       </c>
       <c r="J3"/>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L3"/>
-      <c r="M3" t="n">
-        <v>10.0</v>
+      <c r="M3" t="s">
+        <v>24</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="O3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3.0</v>
+        <v>102.0</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C4" t="n">
-        <v>2017.0</v>
+        <v>2020.0</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="J4"/>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
       <c r="K4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="L4"/>
-      <c r="M4" t="n">
-        <v>10.0</v>
+      <c r="M4" t="s">
+        <v>24</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="O4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="P4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4.0</v>
+        <v>103.0</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C5" t="n">
-        <v>2015.0</v>
+        <v>2020.0</v>
       </c>
       <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
         <v>40</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
       </c>
       <c r="I5" t="s">
         <v>22</v>
       </c>
-      <c r="J5"/>
-      <c r="K5"/>
+      <c r="J5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" t="s">
+        <v>43</v>
+      </c>
       <c r="L5"/>
-      <c r="M5" t="n">
-        <v>14.0</v>
+      <c r="M5" t="s">
+        <v>24</v>
       </c>
       <c r="N5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>201.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2020.0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
         <v>40</v>
       </c>
-      <c r="O5" t="s">
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6"/>
+      <c r="M6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" t="s">
         <v>44</v>
       </c>
-      <c r="P5" t="s">
+      <c r="O6" t="s">
         <v>45</v>
+      </c>
+      <c r="P6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>202.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2020.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7"/>
+      <c r="M7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" t="s">
+        <v>45</v>
+      </c>
+      <c r="P7" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>